<commit_message>
Modified timeline with proposed goal dates
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Timeline</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Accomplished</t>
+  </si>
+  <si>
+    <t>Who should do what?</t>
   </si>
   <si>
     <t xml:space="preserve">Look up and research NLP tools. Look for libraries. Research ways to store data to files so we don’t have to build every time. </t>
@@ -168,6 +171,9 @@
     <xf numFmtId="0" fontId="1" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -175,9 +181,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -231,7 +234,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozenSplit"/>
@@ -243,7 +246,8 @@
     <col min="2" max="2" width="45.9375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.05469" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.2891" style="1" customWidth="1"/>
-    <col min="5" max="256" width="9.05469" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.9531" style="1" customWidth="1"/>
+    <col min="6" max="256" width="9.05469" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.55" customHeight="1">
@@ -259,192 +263,230 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" ht="32.55" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="C2" s="5">
+        <v>40230</v>
+      </c>
       <c r="D2" s="4"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" ht="32.35" customHeight="1">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="C3" s="5">
+        <v>40230</v>
+      </c>
       <c r="D3" s="4"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="6">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5"/>
+      <c r="B4" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5">
+        <v>40233</v>
+      </c>
       <c r="D4" s="4"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="C5" s="5">
+        <v>40237</v>
+      </c>
       <c r="D5" s="4"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="C6" s="5">
+        <v>40244</v>
+      </c>
       <c r="D6" s="4"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="C7" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C7" s="5">
+        <v>40251</v>
+      </c>
       <c r="D7" s="4"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>10</v>
-      </c>
-      <c r="C8" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="C8" s="5">
+        <v>40258</v>
+      </c>
       <c r="D8" s="4"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="7">
-        <v>11</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="B9" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5">
         <v>40268</v>
       </c>
       <c r="D9" s="4"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="4"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="4"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" ht="20.35" customHeight="1">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="4"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="4"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="4"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="4"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="4"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" ht="20.35" customHeight="1">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="4"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" ht="20.35" customHeight="1">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="4"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" ht="20.35" customHeight="1">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="4"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" ht="20.35" customHeight="1">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="4"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" ht="20.35" customHeight="1">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
+      <c r="C21" s="6"/>
       <c r="D21" s="4"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" ht="20.35" customHeight="1">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
+      <c r="C22" s="6"/>
       <c r="D22" s="4"/>
+      <c r="E22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -480,10 +522,10 @@
     <row r="1" ht="2" customHeight="1"/>
     <row r="2" ht="20.55" customHeight="1">
       <c r="B2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -493,10 +535,10 @@
       <c r="B3" s="11">
         <v>40230</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
       <c r="B4" s="12"/>
@@ -507,10 +549,10 @@
     </row>
     <row r="5" ht="20.35" customHeight="1">
       <c r="B5" s="12"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
       <c r="B6" s="12"/>
@@ -521,10 +563,10 @@
     </row>
     <row r="7" ht="20.35" customHeight="1">
       <c r="B7" s="12"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
       <c r="B8" s="12"/>
@@ -535,10 +577,10 @@
     </row>
     <row r="9" ht="20.35" customHeight="1">
       <c r="B9" s="12"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
       <c r="B10" s="12"/>
@@ -549,10 +591,10 @@
     </row>
     <row r="11" ht="20.35" customHeight="1">
       <c r="B11" s="12"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -586,7 +628,7 @@
     <row r="1" ht="2" customHeight="1"/>
     <row r="2" ht="20.55" customHeight="1">
       <c r="B2" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -594,21 +636,21 @@
     <row r="3" ht="32.55" customHeight="1">
       <c r="B3" s="12"/>
       <c r="C3" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
       <c r="B4" s="12"/>
       <c r="C4" t="s" s="15">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="13"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
       <c r="B5" s="12"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
       <c r="B6" s="12"/>
@@ -617,8 +659,8 @@
     </row>
     <row r="7" ht="20.35" customHeight="1">
       <c r="B7" s="12"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
       <c r="B8" s="12"/>
@@ -627,8 +669,8 @@
     </row>
     <row r="9" ht="20.35" customHeight="1">
       <c r="B9" s="12"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
       <c r="B10" s="12"/>
@@ -637,8 +679,8 @@
     </row>
     <row r="11" ht="20.35" customHeight="1">
       <c r="B11" s="12"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
Added Excel version of timeline
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -10,12 +10,13 @@
     <sheet name="Checklist" sheetId="2" r:id="rId4"/>
     <sheet name="Timesheet" sheetId="3" r:id="rId5"/>
     <sheet name="Ideas" sheetId="4" r:id="rId6"/>
+    <sheet name="Question" sheetId="5" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>Timeline</t>
   </si>
@@ -53,7 +54,22 @@
     <t>COMPLETE PROJECT</t>
   </si>
   <si>
-    <t>Parse article files</t>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Who?</t>
+  </si>
+  <si>
+    <t>Date accomplished</t>
+  </si>
+  <si>
+    <t>Parse article files (HTML)</t>
+  </si>
+  <si>
+    <t>Eric Gan</t>
+  </si>
+  <si>
+    <t>Categorize question difficulty</t>
   </si>
   <si>
     <t>Date</t>
@@ -62,6 +78,12 @@
     <t>Things we accomplished</t>
   </si>
   <si>
+    <t>Downloaded NLTK</t>
+  </si>
+  <si>
+    <t>Researched NLTK and its module for POS tagging</t>
+  </si>
+  <si>
     <t>Ideas</t>
   </si>
   <si>
@@ -83,6 +105,12 @@
     <t>dict to .csv and back for Python (Aaron)</t>
   </si>
   <si>
+    <t>Questions that might have a dependent clause appended to it.</t>
+  </si>
+  <si>
+    <t>Ignore them for now</t>
+  </si>
+  <si>
     <t>How to store the article files when we train our model.</t>
   </si>
   <si>
@@ -90,6 +118,15 @@
   </si>
   <si>
     <t>First, parse sentence. Then convert to 3-grams.</t>
+  </si>
+  <si>
+    <t>Are we able to use/install nltk?</t>
+  </si>
+  <si>
+    <t>What is our data limit (in size)?</t>
+  </si>
+  <si>
+    <t>We need to install nltk_data onto linux machines.</t>
   </si>
 </sst>
 </file>
@@ -177,7 +214,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -211,22 +248,28 @@
     <xf numFmtId="0" fontId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -536,7 +579,7 @@
     <col min="1" max="1" width="0.25" style="10" customWidth="1"/>
     <col min="2" max="2" width="13.9219" style="10" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="10" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="10" customWidth="1"/>
+    <col min="4" max="4" width="15.1328" style="10" customWidth="1"/>
     <col min="5" max="5" width="12.25" style="10" customWidth="1"/>
     <col min="6" max="6" width="12.25" style="10" customWidth="1"/>
     <col min="7" max="256" width="12.25" style="10" customWidth="1"/>
@@ -544,22 +587,32 @@
   <sheetData>
     <row r="1" ht="2" customHeight="1"/>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>14</v>
+      </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="B3" s="11"/>
-      <c r="C3" s="7"/>
+    <row r="3" ht="32.55" customHeight="1">
+      <c r="B3" t="s" s="11">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>16</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" ht="20.35" customHeight="1">
+    <row r="4" ht="32.35" customHeight="1">
       <c r="B4" t="s" s="4">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -567,49 +620,49 @@
       <c r="F4" s="12"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="B5" s="11"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="B7" s="11"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="B8" s="11"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="B9" s="11"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="B10" s="11"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -637,87 +690,91 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="0.25" style="13" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="13" customWidth="1"/>
-    <col min="3" max="3" width="20.9062" style="13" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="13" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="13" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="13" customWidth="1"/>
-    <col min="7" max="256" width="12.25" style="13" customWidth="1"/>
+    <col min="1" max="1" width="0.25" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="14" customWidth="1"/>
+    <col min="3" max="3" width="37.1328" style="14" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="14" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="14" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="14" customWidth="1"/>
+    <col min="7" max="256" width="12.25" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="2" customHeight="1"/>
     <row r="2" ht="20.55" customHeight="1">
       <c r="B2" t="s" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" ht="20.55" customHeight="1">
-      <c r="B3" s="14">
+      <c r="B3" s="15">
         <v>40230</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" t="s" s="5">
+        <v>20</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" t="s" s="16">
+        <v>21</v>
+      </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="B5" s="11"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="B7" s="11"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="B8" s="11"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="B9" s="11"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="B10" s="11"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -745,94 +802,206 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="0.25" style="15" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="15" customWidth="1"/>
-    <col min="3" max="3" width="56.1719" style="15" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="15" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="15" customWidth="1"/>
-    <col min="6" max="256" width="12.25" style="15" customWidth="1"/>
+    <col min="1" max="1" width="0.25" style="17" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="17" customWidth="1"/>
+    <col min="3" max="3" width="56.1719" style="17" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="17" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="17" customWidth="1"/>
+    <col min="6" max="256" width="12.25" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="2" customHeight="1"/>
     <row r="2" ht="20.55" customHeight="1">
       <c r="B2" s="3"/>
       <c r="C2" t="s" s="2">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" ht="32.55" customHeight="1">
-      <c r="B3" s="11"/>
+      <c r="B3" s="13"/>
       <c r="C3" t="s" s="5">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="B4" s="11"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" ht="56.35" customHeight="1">
+      <c r="B4" s="13"/>
       <c r="C4" t="s" s="16">
-        <v>21</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+        <v>28</v>
+      </c>
+      <c r="D4" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s" s="16">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="B5" s="11"/>
+      <c r="B5" s="13"/>
       <c r="C5" t="s" s="5">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
       <c r="B6" t="s" s="4">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s" s="16">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="B7" s="11"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="B8" s="11"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="B9" s="11"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="B10" s="11"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;"Helvetica,Regular"&amp;11&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="0.25" style="18" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="18" customWidth="1"/>
+    <col min="3" max="3" width="30.4062" style="18" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="18" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="18" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="18" customWidth="1"/>
+    <col min="7" max="256" width="12.25" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="2" customHeight="1"/>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" ht="20.55" customHeight="1">
+      <c r="B3" s="13"/>
+      <c r="C3" t="s" s="5">
+        <v>34</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="B4" s="13"/>
+      <c r="C4" t="s" s="16">
+        <v>35</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="B5" s="13"/>
+      <c r="C5" t="s" s="5">
+        <v>36</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="B6" s="13"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" ht="20.35" customHeight="1">
+      <c r="B7" s="13"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" ht="20.35" customHeight="1">
+      <c r="B8" s="13"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="B9" s="13"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="B10" s="13"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="B11" s="13"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>